<commit_message>
Dataset Collected for temp and humidity
</commit_message>
<xml_diff>
--- a/datasave.xlsx
+++ b/datasave.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{05922318-A65C-4ECA-82ED-A337301EE580}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2EF53086-56B1-4EA9-A105-85D2AECA4507}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -343,10 +343,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B151"/>
+  <dimension ref="A1:B266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="A151" sqref="A151"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="C177" sqref="C177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1552,10 +1552,930 @@
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+      <c r="A151">
+        <v>27</v>
+      </c>
+      <c r="B151">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>27</v>
+      </c>
+      <c r="B152">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>27</v>
+      </c>
+      <c r="B153">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>27</v>
+      </c>
+      <c r="B154">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>27</v>
+      </c>
+      <c r="B155">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>27</v>
+      </c>
+      <c r="B156">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>27</v>
+      </c>
+      <c r="B157">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>27</v>
+      </c>
+      <c r="B158">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>27</v>
+      </c>
+      <c r="B159">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>27</v>
+      </c>
+      <c r="B160">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>27</v>
+      </c>
+      <c r="B161">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>27</v>
+      </c>
+      <c r="B162">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>27</v>
+      </c>
+      <c r="B163">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>27</v>
+      </c>
+      <c r="B164">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>27</v>
+      </c>
+      <c r="B165">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>27</v>
+      </c>
+      <c r="B166">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>27</v>
+      </c>
+      <c r="B167">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>27</v>
+      </c>
+      <c r="B168">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>27</v>
+      </c>
+      <c r="B169">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>27</v>
+      </c>
+      <c r="B170">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>27</v>
+      </c>
+      <c r="B171">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>27</v>
+      </c>
+      <c r="B172">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>27</v>
+      </c>
+      <c r="B173">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>27</v>
+      </c>
+      <c r="B174">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>27</v>
+      </c>
+      <c r="B175">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>27</v>
+      </c>
+      <c r="B176">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>25</v>
+      </c>
+      <c r="B177">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>25</v>
+      </c>
+      <c r="B178">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>25</v>
+      </c>
+      <c r="B179">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>25</v>
+      </c>
+      <c r="B180">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>25</v>
+      </c>
+      <c r="B181">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>25</v>
+      </c>
+      <c r="B182">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>25</v>
+      </c>
+      <c r="B183">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>25</v>
+      </c>
+      <c r="B184">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>25</v>
+      </c>
+      <c r="B185">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>25</v>
+      </c>
+      <c r="B186">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>25</v>
+      </c>
+      <c r="B187">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>25</v>
+      </c>
+      <c r="B188">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>25</v>
+      </c>
+      <c r="B189">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>25</v>
+      </c>
+      <c r="B190">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>25</v>
+      </c>
+      <c r="B191">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>25</v>
+      </c>
+      <c r="B192">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>25</v>
+      </c>
+      <c r="B193">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>25</v>
+      </c>
+      <c r="B194">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>25</v>
+      </c>
+      <c r="B195">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>25</v>
+      </c>
+      <c r="B196">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>25</v>
+      </c>
+      <c r="B197">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>25</v>
+      </c>
+      <c r="B198">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>25</v>
+      </c>
+      <c r="B199">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>25</v>
+      </c>
+      <c r="B200">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>25</v>
+      </c>
+      <c r="B201">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>25</v>
+      </c>
+      <c r="B202">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>25</v>
+      </c>
+      <c r="B203">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>25</v>
+      </c>
+      <c r="B204">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>25</v>
+      </c>
+      <c r="B205">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>25</v>
+      </c>
+      <c r="B206">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>25</v>
+      </c>
+      <c r="B207">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>25</v>
+      </c>
+      <c r="B208">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>25</v>
+      </c>
+      <c r="B209">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>25</v>
+      </c>
+      <c r="B210">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>25</v>
+      </c>
+      <c r="B211">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>25</v>
+      </c>
+      <c r="B212">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>25</v>
+      </c>
+      <c r="B213">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>25</v>
+      </c>
+      <c r="B214">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>25</v>
+      </c>
+      <c r="B215">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>25</v>
+      </c>
+      <c r="B216">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>25</v>
+      </c>
+      <c r="B217">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>25</v>
+      </c>
+      <c r="B218">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>25</v>
+      </c>
+      <c r="B219">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>25</v>
+      </c>
+      <c r="B220">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>25</v>
+      </c>
+      <c r="B221">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>25</v>
+      </c>
+      <c r="B222">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>25</v>
+      </c>
+      <c r="B223">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>25</v>
+      </c>
+      <c r="B224">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>25</v>
+      </c>
+      <c r="B225">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>25</v>
+      </c>
+      <c r="B226">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>25</v>
+      </c>
+      <c r="B227">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>25</v>
+      </c>
+      <c r="B228">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>25</v>
+      </c>
+      <c r="B229">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>25</v>
+      </c>
+      <c r="B230">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>25</v>
+      </c>
+      <c r="B231">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>25</v>
+      </c>
+      <c r="B232">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>25</v>
+      </c>
+      <c r="B233">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>25</v>
+      </c>
+      <c r="B234">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>25</v>
+      </c>
+      <c r="B235">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>25</v>
+      </c>
+      <c r="B236">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>25</v>
+      </c>
+      <c r="B237">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>25</v>
+      </c>
+      <c r="B238">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>25</v>
+      </c>
+      <c r="B239">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>25</v>
+      </c>
+      <c r="B240">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>25</v>
+      </c>
+      <c r="B241">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>25</v>
+      </c>
+      <c r="B242">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>25</v>
+      </c>
+      <c r="B243">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>25</v>
+      </c>
+      <c r="B244">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>25</v>
+      </c>
+      <c r="B245">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>25</v>
+      </c>
+      <c r="B246">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>25</v>
+      </c>
+      <c r="B247">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>25</v>
+      </c>
+      <c r="B248">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>25</v>
+      </c>
+      <c r="B249">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>25</v>
+      </c>
+      <c r="B250">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>25</v>
+      </c>
+      <c r="B251">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>25</v>
+      </c>
+      <c r="B252">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>25</v>
+      </c>
+      <c r="B253">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>25</v>
+      </c>
+      <c r="B254">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>25</v>
+      </c>
+      <c r="B255">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>25</v>
+      </c>
+      <c r="B256">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>25</v>
+      </c>
+      <c r="B257">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>25</v>
+      </c>
+      <c r="B258">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>25</v>
+      </c>
+      <c r="B259">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>25</v>
+      </c>
+      <c r="B260">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>25</v>
+      </c>
+      <c r="B261">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>25</v>
+      </c>
+      <c r="B262">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>25</v>
+      </c>
+      <c r="B263">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>25</v>
+      </c>
+      <c r="B264">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>25</v>
+      </c>
+      <c r="B265">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
         <v>1</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B266" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>